<commit_message>
3predict:grafici: modificati grafici di excel
</commit_message>
<xml_diff>
--- a/3predict/Grafici/Accuracy, Loss.xlsx
+++ b/3predict/Grafici/Accuracy, Loss.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniudamce-my.sharepoint.com/personal/142985_spes_uniud_it/Documents/Magistrale/1. Deep Learning/Progetti/Progetto_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\flutter_pro\multi-object-detection\3predict\Grafici\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_F25DC773A252ABDACC104857891B614C5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{114F489B-A33C-4202-A909-8CB8D8377884}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E78EE3-3F6E-482B-84AD-8F4D5CB3D186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -6438,7 +6438,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -20977,8 +20977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136A544A-A6CE-4DE3-9206-844A3454B298}">
   <dimension ref="A1:E2002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>